<commit_message>
converted forest area to percentage
</commit_message>
<xml_diff>
--- a/Project/Datasets/forestareadiffcountries.xlsx
+++ b/Project/Datasets/forestareadiffcountries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarthak/Desktop/IIIT Course Work/Sem4/Data Visulisation/DataVisualisation/Project/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EA8FAA6-D4B2-3943-A30A-04B4BF6E3321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978A2FC2-19FB-F44C-B5A5-F5DFF88B77AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="500" windowWidth="27640" windowHeight="15580" xr2:uid="{E6B63C7C-647E-3947-B082-3B3CA17A01F1}"/>
+    <workbookView xWindow="9260" yWindow="500" windowWidth="27640" windowHeight="15580" xr2:uid="{E6B63C7C-647E-3947-B082-3B3CA17A01F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Australia</t>
   </si>
@@ -69,12 +69,18 @@
   <si>
     <t>Democratic Republic of Congo</t>
   </si>
+  <si>
+    <t xml:space="preserve">	9,826,675</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,6 +98,12 @@
     <font>
       <sz val="12"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,10 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,18 +446,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4033245-FE24-8642-8565-1AD96C3624ED}">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="59.1640625" customWidth="1"/>
+    <col min="33" max="33" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -540,8 +555,11 @@
       <c r="AF1">
         <v>2020</v>
       </c>
+      <c r="AG1" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -638,8 +656,11 @@
       <c r="AF2">
         <v>1340051</v>
       </c>
+      <c r="AG2">
+        <v>7692020</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -736,8 +757,11 @@
       <c r="AF3">
         <v>8153116</v>
       </c>
+      <c r="AG3" s="3">
+        <v>16376870</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -834,8 +858,11 @@
       <c r="AF4">
         <v>4966196</v>
       </c>
+      <c r="AG4" s="3">
+        <v>8515767</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -932,8 +959,11 @@
       <c r="AF5">
         <v>3469281</v>
       </c>
+      <c r="AG5" s="3">
+        <v>9879750</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1030,8 +1060,11 @@
       <c r="AF6">
         <v>3097950</v>
       </c>
+      <c r="AG6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1128,8 +1161,11 @@
       <c r="AF7">
         <v>2199781.7999999998</v>
       </c>
+      <c r="AG7">
+        <v>9600000</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1226,8 +1262,11 @@
       <c r="AF8">
         <v>1261552.3999999999</v>
       </c>
+      <c r="AG8" s="3">
+        <v>2344858</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1324,8 +1363,11 @@
       <c r="AF9">
         <v>921332</v>
       </c>
+      <c r="AG9" s="3">
+        <v>1904569</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1422,8 +1464,11 @@
       <c r="AF10">
         <v>723303.7</v>
       </c>
+      <c r="AG10" s="3">
+        <v>1285082</v>
+      </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1519,6 +1564,9 @@
       </c>
       <c r="AF11">
         <v>721600</v>
+      </c>
+      <c r="AG11">
+        <v>3287263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>